<commit_message>
updated script and calibration for exo wage
</commit_message>
<xml_diff>
--- a/julia/Parameterizations/calibration_Nov4.xlsx
+++ b/julia/Parameterizations/calibration_Nov4.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\Research\Teachers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Documents\GitHub\teachers\julia\Parameterizations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4477C44-9CAD-4C67-81FC-5730DB55DE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C2A543-E39C-49C8-ABA8-437F49F6E9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-15" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="2" r:id="rId1"/>
     <sheet name="occ_shares" sheetId="4" r:id="rId2"/>
     <sheet name="compar_stat" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="143">
   <si>
     <t>output</t>
   </si>
@@ -447,6 +448,27 @@
   </si>
   <si>
     <t>[-0.4050; -0.1564]</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>Frechet(theta)</t>
+  </si>
+  <si>
+    <t>h is less than 1</t>
+  </si>
+  <si>
+    <t>kappa</t>
+  </si>
+  <si>
+    <t>kappa*h^gamma</t>
+  </si>
+  <si>
+    <t>lambda_female (scale of tau rel to T)</t>
+  </si>
+  <si>
+    <t>lambda_male (scale of tau rel to T)</t>
   </si>
 </sst>
 </file>
@@ -523,7 +545,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -545,6 +567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -877,7 +900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE97B36E-EB7E-41AB-A80A-B97BDD0CFFC5}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
@@ -1851,7 +1874,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG42" sqref="AG42"/>
+      <selection pane="bottomRight" activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4789,4 +4812,615 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E39CD9E-1C94-476B-AB01-C44D77640615}">
+  <dimension ref="A1:G51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="C2">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="D2">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="E2">
+        <v>8.8999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="E3">
+        <v>0.10299999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>0.999</v>
+      </c>
+      <c r="C4">
+        <v>0.999</v>
+      </c>
+      <c r="D4">
+        <v>0.999</v>
+      </c>
+      <c r="E4">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="C5">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="D5">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="E5">
+        <v>0.71399999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>2010</v>
+      </c>
+      <c r="C9">
+        <v>2010</v>
+      </c>
+      <c r="D9">
+        <v>2010</v>
+      </c>
+      <c r="E9">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11">
+        <v>2010</v>
+      </c>
+      <c r="C11">
+        <v>2010</v>
+      </c>
+      <c r="D11">
+        <v>2010</v>
+      </c>
+      <c r="E11">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E12">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="17">
+        <v>3.7691675988456602E-6</v>
+      </c>
+      <c r="C20">
+        <v>0.14871198773538699</v>
+      </c>
+      <c r="D20">
+        <v>2.1262390644812699E-2</v>
+      </c>
+      <c r="E20" s="17">
+        <v>4.7514101157888599E-6</v>
+      </c>
+      <c r="G20" s="17"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21">
+        <v>3.74181457780348E-3</v>
+      </c>
+      <c r="C21">
+        <v>0.77080826898398902</v>
+      </c>
+      <c r="D21">
+        <v>0.29537392832944698</v>
+      </c>
+      <c r="E21">
+        <v>4.4936918354969903E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22">
+        <v>270.73201588421699</v>
+      </c>
+      <c r="C22">
+        <v>1.1183336013305301</v>
+      </c>
+      <c r="D22">
+        <v>3.33467398200942</v>
+      </c>
+      <c r="E22">
+        <v>227.026454379021</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24">
+        <v>0.997258825868933</v>
+      </c>
+      <c r="C24">
+        <v>0.85746306715555098</v>
+      </c>
+      <c r="D24">
+        <v>0.97591184715801105</v>
+      </c>
+      <c r="E24">
+        <v>0.99798579618518601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25">
+        <v>0.99422785112084</v>
+      </c>
+      <c r="C25">
+        <v>0.56009268914888299</v>
+      </c>
+      <c r="D25">
+        <v>0.76432993244089997</v>
+      </c>
+      <c r="E25">
+        <v>0.99354979688447898</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="17">
+        <v>1.2337512032765601E-5</v>
+      </c>
+      <c r="C26">
+        <v>3.8438956827681098E-3</v>
+      </c>
+      <c r="D26">
+        <v>2.1283278161620899E-3</v>
+      </c>
+      <c r="E26" s="17">
+        <v>1.59453439331234E-5</v>
+      </c>
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="17">
+        <v>1.18821631625977E-5</v>
+      </c>
+      <c r="C27">
+        <v>3.58980397830426E-3</v>
+      </c>
+      <c r="D27">
+        <v>1.9013358603460599E-3</v>
+      </c>
+      <c r="E27" s="17">
+        <v>1.5278695135325199E-5</v>
+      </c>
+      <c r="G27" s="17"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28">
+        <v>0.44295609599785302</v>
+      </c>
+      <c r="C28">
+        <v>0.414364585252263</v>
+      </c>
+      <c r="D28">
+        <v>0.42893647227634202</v>
+      </c>
+      <c r="E28" s="17">
+        <v>0.44569650152129803</v>
+      </c>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29">
+        <v>0.44295609599785302</v>
+      </c>
+      <c r="C29">
+        <v>0.414364585252263</v>
+      </c>
+      <c r="D29">
+        <v>0.42893647227634202</v>
+      </c>
+      <c r="E29">
+        <v>0.44569650152129803</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30">
+        <v>1.20004091486983E-4</v>
+      </c>
+      <c r="C30">
+        <v>7.7552304471485797E-2</v>
+      </c>
+      <c r="D30">
+        <v>2.5856085963030601E-2</v>
+      </c>
+      <c r="E30">
+        <v>1.5361957258571099E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31">
+        <v>1.1557501961827799E-4</v>
+      </c>
+      <c r="C31">
+        <v>7.2425891359757202E-2</v>
+      </c>
+      <c r="D31">
+        <v>2.3098464003703301E-2</v>
+      </c>
+      <c r="E31">
+        <v>1.4719698905210599E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35">
+        <v>0.44295609599785302</v>
+      </c>
+      <c r="C35">
+        <v>0.44295609599785302</v>
+      </c>
+      <c r="D35">
+        <v>0.44295609599785302</v>
+      </c>
+      <c r="E35">
+        <v>0.44295609599785302</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36">
+        <v>0.44295609599785302</v>
+      </c>
+      <c r="C36">
+        <v>0.44295609599785302</v>
+      </c>
+      <c r="D36">
+        <v>0.44295609599785302</v>
+      </c>
+      <c r="E36">
+        <v>0.44295609599785302</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>1.8702968764208001E-3</v>
+      </c>
+      <c r="C38">
+        <v>0.46536833952368001</v>
+      </c>
+      <c r="D38">
+        <v>0.15898785552165801</v>
+      </c>
+      <c r="E38">
+        <v>2.2702471490636E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>2.3086322133876401E-4</v>
+      </c>
+      <c r="C39">
+        <v>7.7339713538861696E-2</v>
+      </c>
+      <c r="D39">
+        <v>3.8978500709643697E-2</v>
+      </c>
+      <c r="E39">
+        <v>2.9042210533849398E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" s="17">
+        <v>2.1753902132322099E-7</v>
+      </c>
+      <c r="C40">
+        <v>2.51485334579706E-2</v>
+      </c>
+      <c r="D40">
+        <v>3.01960881956779E-3</v>
+      </c>
+      <c r="E40" s="17">
+        <v>3.2887347778848499E-7</v>
+      </c>
+      <c r="G40" s="17"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
clean up versions of code and manuscript
</commit_message>
<xml_diff>
--- a/julia/Parameterizations/calibration_Nov4.xlsx
+++ b/julia/Parameterizations/calibration_Nov4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Documents\GitHub\teachers\julia\Parameterizations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9199B90-008A-42C7-891E-E19B951A32F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABC21C1-2F85-4603-93ED-43452F43787C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-15" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="occ_shares" sheetId="4" r:id="rId2"/>
     <sheet name="compar_stat" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
+    <sheet name="exo_wage" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4818,8 +4818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E39CD9E-1C94-476B-AB01-C44D77640615}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>